<commit_message>
12 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$481</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1854,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="B173" sqref="B173"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3701,7 +3704,7 @@
         <v>172</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="21">
@@ -3723,7 +3726,7 @@
         <v>174</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="21">
@@ -3745,7 +3748,7 @@
         <v>176</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="21">
@@ -3756,7 +3759,7 @@
         <v>177</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="21">
@@ -3767,7 +3770,7 @@
         <v>178</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="21">
@@ -3778,7 +3781,7 @@
         <v>179</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="21">
@@ -4989,7 +4992,7 @@
         <v>289</v>
       </c>
       <c r="C299" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="300" spans="1:3" ht="21">
@@ -7375,5 +7378,6 @@
     <hyperlink ref="B2" r:id="rId446"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId447"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
19 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1858,7 +1858,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3403,7 +3403,7 @@
         <v>144</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="21">
@@ -3715,7 +3715,7 @@
         <v>173</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="21">
@@ -3792,7 +3792,7 @@
         <v>180</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="21">
@@ -3803,7 +3803,7 @@
         <v>181</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="21">
@@ -3814,7 +3814,7 @@
         <v>182</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="21">
@@ -3825,7 +3825,7 @@
         <v>183</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="21">
@@ -3836,7 +3836,7 @@
         <v>184</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="21">

</xml_diff>

<commit_message>
24 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A183" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B196" sqref="B196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2166,7 +2166,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="21">
@@ -2701,7 +2701,7 @@
         <v>79</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="21">
@@ -2756,7 +2756,7 @@
         <v>84</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="21">
@@ -3359,7 +3359,7 @@
         <v>140</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="21">
@@ -3891,7 +3891,7 @@
         <v>189</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="21">

</xml_diff>

<commit_message>
29 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B196" sqref="B196"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3946,7 +3946,7 @@
         <v>194</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="21">
@@ -4121,7 +4121,7 @@
         <v>210</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="21">
@@ -4143,7 +4143,7 @@
         <v>212</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="21">
@@ -4220,7 +4220,7 @@
         <v>219</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="226" spans="1:3" ht="21">
@@ -4231,7 +4231,7 @@
         <v>220</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="227" spans="1:3" ht="21">

</xml_diff>

<commit_message>
35 of 450 question done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3634,7 +3634,7 @@
         <v>165</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="21">
@@ -3678,7 +3678,7 @@
         <v>169</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="21">
@@ -3847,7 +3847,7 @@
         <v>185</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="21">
@@ -3968,7 +3968,7 @@
         <v>196</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="21">
@@ -5102,7 +5102,7 @@
         <v>299</v>
       </c>
       <c r="C309" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="310" spans="1:3" ht="21">
@@ -5366,7 +5366,7 @@
         <v>323</v>
       </c>
       <c r="C333" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="334" spans="1:3" ht="21">

</xml_diff>

<commit_message>
39 of 450 quuestions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A238" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1913,7 +1913,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21">
@@ -1924,7 +1924,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21">
@@ -1935,7 +1935,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21">
@@ -2388,7 +2388,7 @@
         <v>50</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="21">

</xml_diff>

<commit_message>
42 of 450 question done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2492,7 +2492,7 @@
         <v>60</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="21">
@@ -2833,7 +2833,7 @@
         <v>91</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="21">
@@ -2981,7 +2981,7 @@
         <v>105</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="21">

</xml_diff>

<commit_message>
44 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A188" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="C206" sqref="C206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3902,7 +3902,7 @@
         <v>190</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="21">
@@ -4023,7 +4023,7 @@
         <v>201</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="207" spans="1:3" ht="21">

</xml_diff>

<commit_message>
49 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A335" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B346" sqref="B346"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2624,7 +2624,7 @@
         <v>72</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="21">
@@ -2888,7 +2888,7 @@
         <v>96</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="21">
@@ -5473,7 +5473,7 @@
         <v>333</v>
       </c>
       <c r="C344" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="345" spans="1:3" ht="21">
@@ -5484,7 +5484,7 @@
         <v>334</v>
       </c>
       <c r="C345" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="346" spans="1:3" ht="21">
@@ -5528,7 +5528,7 @@
         <v>338</v>
       </c>
       <c r="C349" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="350" spans="1:3" ht="21">

</xml_diff>

<commit_message>
52 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A331" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B339" sqref="B339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2712,7 +2712,7 @@
         <v>80</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="21">
@@ -3047,7 +3047,7 @@
         <v>111</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="21">
@@ -3315,7 +3315,7 @@
         <v>136</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="21">

</xml_diff>

<commit_message>
55 of 450 question done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A331" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B339" sqref="B339"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4034,7 +4034,7 @@
         <v>202</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="208" spans="1:3" ht="21">
@@ -4099,7 +4099,7 @@
         <v>208</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="21">
@@ -4165,7 +4165,7 @@
         <v>214</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="21">

</xml_diff>

<commit_message>
58 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1858,7 +1858,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2569,7 +2569,7 @@
         <v>67</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="21">
@@ -2734,7 +2734,7 @@
         <v>82</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="21">
@@ -2904,7 +2904,7 @@
         <v>98</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="21">
@@ -6938,444 +6938,444 @@
     <hyperlink ref="B11" r:id="rId6"/>
     <hyperlink ref="B12" r:id="rId7"/>
     <hyperlink ref="B13" r:id="rId8"/>
-    <hyperlink ref="B14" r:id="rId9"/>
-    <hyperlink ref="B15" r:id="rId10"/>
-    <hyperlink ref="B16" r:id="rId11"/>
-    <hyperlink ref="B17" r:id="rId12"/>
-    <hyperlink ref="B18" r:id="rId13"/>
-    <hyperlink ref="B19" r:id="rId14"/>
-    <hyperlink ref="B20" r:id="rId15"/>
-    <hyperlink ref="B21" r:id="rId16"/>
-    <hyperlink ref="B22" r:id="rId17"/>
-    <hyperlink ref="B23" r:id="rId18"/>
-    <hyperlink ref="B24" r:id="rId19"/>
-    <hyperlink ref="B25" r:id="rId20"/>
-    <hyperlink ref="B26" r:id="rId21"/>
-    <hyperlink ref="B27" r:id="rId22"/>
-    <hyperlink ref="B28" r:id="rId23"/>
-    <hyperlink ref="B29" r:id="rId24"/>
-    <hyperlink ref="B30" r:id="rId25"/>
-    <hyperlink ref="B31" r:id="rId26"/>
-    <hyperlink ref="B32" r:id="rId27"/>
-    <hyperlink ref="B33" r:id="rId28"/>
-    <hyperlink ref="B34" r:id="rId29"/>
-    <hyperlink ref="B35" r:id="rId30"/>
-    <hyperlink ref="B36" r:id="rId31"/>
-    <hyperlink ref="B37" r:id="rId32"/>
-    <hyperlink ref="B38" r:id="rId33"/>
-    <hyperlink ref="B39" r:id="rId34"/>
-    <hyperlink ref="B40" r:id="rId35"/>
-    <hyperlink ref="B41" r:id="rId36"/>
-    <hyperlink ref="B44" r:id="rId37"/>
-    <hyperlink ref="B45" r:id="rId38"/>
-    <hyperlink ref="B46" r:id="rId39"/>
-    <hyperlink ref="B47" r:id="rId40"/>
-    <hyperlink ref="B48" r:id="rId41"/>
-    <hyperlink ref="B49" r:id="rId42"/>
-    <hyperlink ref="B50" r:id="rId43"/>
-    <hyperlink ref="B51" r:id="rId44"/>
-    <hyperlink ref="B52" r:id="rId45"/>
-    <hyperlink ref="B53" r:id="rId46"/>
-    <hyperlink ref="B56" r:id="rId47"/>
-    <hyperlink ref="B57" r:id="rId48"/>
-    <hyperlink ref="B58" r:id="rId49"/>
-    <hyperlink ref="B60" r:id="rId50"/>
-    <hyperlink ref="B61" r:id="rId51"/>
-    <hyperlink ref="B62" r:id="rId52"/>
-    <hyperlink ref="B63" r:id="rId53"/>
-    <hyperlink ref="B64" r:id="rId54"/>
-    <hyperlink ref="B65" r:id="rId55"/>
-    <hyperlink ref="B66" r:id="rId56"/>
-    <hyperlink ref="B67" r:id="rId57"/>
-    <hyperlink ref="B68" r:id="rId58"/>
-    <hyperlink ref="B69" r:id="rId59"/>
-    <hyperlink ref="B70" r:id="rId60"/>
-    <hyperlink ref="B71" r:id="rId61"/>
-    <hyperlink ref="B72" r:id="rId62"/>
-    <hyperlink ref="B73" r:id="rId63"/>
-    <hyperlink ref="B74" r:id="rId64"/>
-    <hyperlink ref="B75" r:id="rId65"/>
-    <hyperlink ref="B76" r:id="rId66"/>
-    <hyperlink ref="B77" r:id="rId67"/>
-    <hyperlink ref="B78" r:id="rId68"/>
-    <hyperlink ref="B79" r:id="rId69"/>
-    <hyperlink ref="B80" r:id="rId70"/>
-    <hyperlink ref="B81" r:id="rId71"/>
-    <hyperlink ref="B82" r:id="rId72"/>
-    <hyperlink ref="B83" r:id="rId73"/>
-    <hyperlink ref="B84" r:id="rId74"/>
-    <hyperlink ref="B85" r:id="rId75"/>
-    <hyperlink ref="B86" r:id="rId76"/>
-    <hyperlink ref="B87" r:id="rId77"/>
-    <hyperlink ref="B88" r:id="rId78"/>
-    <hyperlink ref="B89" r:id="rId79"/>
-    <hyperlink ref="B90" r:id="rId80"/>
-    <hyperlink ref="B91" r:id="rId81"/>
-    <hyperlink ref="B92" r:id="rId82"/>
-    <hyperlink ref="B93" r:id="rId83"/>
-    <hyperlink ref="B94" r:id="rId84"/>
-    <hyperlink ref="B95" r:id="rId85"/>
-    <hyperlink ref="B96" r:id="rId86"/>
-    <hyperlink ref="B97" r:id="rId87"/>
-    <hyperlink ref="B98" r:id="rId88"/>
-    <hyperlink ref="B101" r:id="rId89"/>
-    <hyperlink ref="B102" r:id="rId90"/>
-    <hyperlink ref="B103" r:id="rId91"/>
-    <hyperlink ref="B104" r:id="rId92"/>
-    <hyperlink ref="B106" r:id="rId93" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance."/>
-    <hyperlink ref="B107" r:id="rId94"/>
-    <hyperlink ref="B108" r:id="rId95"/>
-    <hyperlink ref="B109" r:id="rId96"/>
-    <hyperlink ref="B110" r:id="rId97"/>
-    <hyperlink ref="B111" r:id="rId98"/>
-    <hyperlink ref="B113" r:id="rId99"/>
-    <hyperlink ref="B114" r:id="rId100"/>
-    <hyperlink ref="B115" r:id="rId101"/>
-    <hyperlink ref="B116" r:id="rId102"/>
-    <hyperlink ref="B117" r:id="rId103"/>
-    <hyperlink ref="B118" r:id="rId104"/>
-    <hyperlink ref="B119" r:id="rId105"/>
-    <hyperlink ref="B120" r:id="rId106"/>
-    <hyperlink ref="B121" r:id="rId107"/>
-    <hyperlink ref="B122" r:id="rId108"/>
-    <hyperlink ref="B123" r:id="rId109"/>
-    <hyperlink ref="B124" r:id="rId110"/>
-    <hyperlink ref="B125" r:id="rId111"/>
-    <hyperlink ref="B126" r:id="rId112"/>
-    <hyperlink ref="B127" r:id="rId113"/>
-    <hyperlink ref="B128" r:id="rId114"/>
-    <hyperlink ref="B129" r:id="rId115"/>
-    <hyperlink ref="B130" r:id="rId116"/>
-    <hyperlink ref="B131" r:id="rId117"/>
-    <hyperlink ref="B132" r:id="rId118"/>
-    <hyperlink ref="B133" r:id="rId119"/>
-    <hyperlink ref="B134" r:id="rId120"/>
-    <hyperlink ref="B135" r:id="rId121"/>
-    <hyperlink ref="B136" r:id="rId122"/>
-    <hyperlink ref="B105" r:id="rId123"/>
-    <hyperlink ref="B112" r:id="rId124"/>
-    <hyperlink ref="B139" r:id="rId125"/>
-    <hyperlink ref="B140" r:id="rId126"/>
-    <hyperlink ref="B141" r:id="rId127"/>
-    <hyperlink ref="B142" r:id="rId128"/>
-    <hyperlink ref="B143" r:id="rId129"/>
-    <hyperlink ref="B144" r:id="rId130"/>
-    <hyperlink ref="B145" r:id="rId131"/>
-    <hyperlink ref="B146" r:id="rId132"/>
-    <hyperlink ref="B147" r:id="rId133"/>
-    <hyperlink ref="B148" r:id="rId134"/>
-    <hyperlink ref="B149" r:id="rId135"/>
-    <hyperlink ref="B150" r:id="rId136"/>
-    <hyperlink ref="B151" r:id="rId137"/>
-    <hyperlink ref="B152" r:id="rId138"/>
-    <hyperlink ref="B153" r:id="rId139"/>
-    <hyperlink ref="B154" r:id="rId140"/>
-    <hyperlink ref="B155" r:id="rId141"/>
-    <hyperlink ref="B156" r:id="rId142"/>
-    <hyperlink ref="B157" r:id="rId143"/>
-    <hyperlink ref="B158" r:id="rId144"/>
-    <hyperlink ref="B159" r:id="rId145"/>
-    <hyperlink ref="B160" r:id="rId146"/>
-    <hyperlink ref="B161" r:id="rId147"/>
-    <hyperlink ref="B162" r:id="rId148"/>
-    <hyperlink ref="B163" r:id="rId149"/>
-    <hyperlink ref="B166" r:id="rId150"/>
-    <hyperlink ref="B167" r:id="rId151"/>
-    <hyperlink ref="B168" r:id="rId152"/>
-    <hyperlink ref="B169" r:id="rId153"/>
-    <hyperlink ref="B170" r:id="rId154"/>
-    <hyperlink ref="B171" r:id="rId155"/>
-    <hyperlink ref="B172" r:id="rId156"/>
-    <hyperlink ref="B173" r:id="rId157"/>
-    <hyperlink ref="B174" r:id="rId158"/>
-    <hyperlink ref="B177" r:id="rId159"/>
-    <hyperlink ref="B178" r:id="rId160"/>
-    <hyperlink ref="B179" r:id="rId161"/>
-    <hyperlink ref="B180" r:id="rId162"/>
-    <hyperlink ref="B181" r:id="rId163"/>
-    <hyperlink ref="B182" r:id="rId164"/>
-    <hyperlink ref="B183" r:id="rId165"/>
-    <hyperlink ref="B184" r:id="rId166"/>
-    <hyperlink ref="B185" r:id="rId167"/>
-    <hyperlink ref="B186" r:id="rId168"/>
-    <hyperlink ref="B187" r:id="rId169"/>
-    <hyperlink ref="B188" r:id="rId170"/>
-    <hyperlink ref="B189" r:id="rId171"/>
-    <hyperlink ref="B190" r:id="rId172"/>
-    <hyperlink ref="B191" r:id="rId173"/>
-    <hyperlink ref="B192" r:id="rId174"/>
-    <hyperlink ref="B193" r:id="rId175"/>
-    <hyperlink ref="B194" r:id="rId176"/>
-    <hyperlink ref="B195" r:id="rId177"/>
-    <hyperlink ref="B196" r:id="rId178"/>
-    <hyperlink ref="B197" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010."/>
-    <hyperlink ref="B198" r:id="rId180"/>
-    <hyperlink ref="B199" r:id="rId181"/>
-    <hyperlink ref="B200" r:id="rId182"/>
-    <hyperlink ref="B201" r:id="rId183"/>
-    <hyperlink ref="B202" r:id="rId184"/>
-    <hyperlink ref="B203" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not."/>
-    <hyperlink ref="B204" r:id="rId186"/>
-    <hyperlink ref="B205" r:id="rId187"/>
-    <hyperlink ref="B206" r:id="rId188"/>
-    <hyperlink ref="B207" r:id="rId189"/>
-    <hyperlink ref="B208" r:id="rId190"/>
-    <hyperlink ref="B209" r:id="rId191"/>
-    <hyperlink ref="B210" r:id="rId192"/>
-    <hyperlink ref="B211" r:id="rId193"/>
-    <hyperlink ref="B214" r:id="rId194"/>
-    <hyperlink ref="B215" r:id="rId195"/>
-    <hyperlink ref="B216" r:id="rId196"/>
-    <hyperlink ref="B217" r:id="rId197"/>
-    <hyperlink ref="B218" r:id="rId198"/>
-    <hyperlink ref="B219" r:id="rId199"/>
-    <hyperlink ref="B220" r:id="rId200"/>
-    <hyperlink ref="B221" r:id="rId201"/>
-    <hyperlink ref="B222" r:id="rId202"/>
-    <hyperlink ref="B223" r:id="rId203"/>
-    <hyperlink ref="B224" r:id="rId204"/>
-    <hyperlink ref="B225" r:id="rId205"/>
-    <hyperlink ref="B226" r:id="rId206"/>
-    <hyperlink ref="B227" r:id="rId207"/>
-    <hyperlink ref="B228" r:id="rId208"/>
-    <hyperlink ref="B229" r:id="rId209"/>
-    <hyperlink ref="B230" r:id="rId210"/>
-    <hyperlink ref="B231" r:id="rId211"/>
-    <hyperlink ref="B232" r:id="rId212"/>
-    <hyperlink ref="B233" r:id="rId213"/>
-    <hyperlink ref="B234" r:id="rId214"/>
-    <hyperlink ref="B235" r:id="rId215"/>
-    <hyperlink ref="B238" r:id="rId216"/>
-    <hyperlink ref="B239" r:id="rId217"/>
-    <hyperlink ref="B240" r:id="rId218"/>
-    <hyperlink ref="B241" r:id="rId219"/>
-    <hyperlink ref="B242" r:id="rId220"/>
-    <hyperlink ref="B243" r:id="rId221"/>
-    <hyperlink ref="B244" r:id="rId222"/>
-    <hyperlink ref="B245" r:id="rId223"/>
-    <hyperlink ref="B246" r:id="rId224"/>
-    <hyperlink ref="B247" r:id="rId225"/>
-    <hyperlink ref="B248" r:id="rId226"/>
-    <hyperlink ref="B249" r:id="rId227"/>
-    <hyperlink ref="B250" r:id="rId228"/>
-    <hyperlink ref="B251" r:id="rId229"/>
-    <hyperlink ref="B252" r:id="rId230"/>
-    <hyperlink ref="B253" r:id="rId231"/>
-    <hyperlink ref="B254" r:id="rId232"/>
-    <hyperlink ref="B255" r:id="rId233"/>
-    <hyperlink ref="B256" r:id="rId234"/>
-    <hyperlink ref="B257" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
-    <hyperlink ref="B258" r:id="rId236"/>
-    <hyperlink ref="B259" r:id="rId237"/>
-    <hyperlink ref="B260" r:id="rId238"/>
-    <hyperlink ref="B261" r:id="rId239"/>
-    <hyperlink ref="B262" r:id="rId240"/>
-    <hyperlink ref="B263" r:id="rId241"/>
-    <hyperlink ref="B264" r:id="rId242"/>
-    <hyperlink ref="B265" r:id="rId243"/>
-    <hyperlink ref="B266" r:id="rId244"/>
-    <hyperlink ref="B267" r:id="rId245"/>
-    <hyperlink ref="B268" r:id="rId246"/>
-    <hyperlink ref="B269" r:id="rId247"/>
-    <hyperlink ref="B270" r:id="rId248"/>
-    <hyperlink ref="B271" r:id="rId249"/>
-    <hyperlink ref="B272" r:id="rId250"/>
-    <hyperlink ref="B275" r:id="rId251"/>
-    <hyperlink ref="B276" r:id="rId252"/>
-    <hyperlink ref="B277" r:id="rId253"/>
-    <hyperlink ref="B278" r:id="rId254"/>
-    <hyperlink ref="B279" r:id="rId255"/>
-    <hyperlink ref="B280" r:id="rId256"/>
-    <hyperlink ref="B281" r:id="rId257"/>
-    <hyperlink ref="B282" r:id="rId258"/>
-    <hyperlink ref="B283" r:id="rId259"/>
-    <hyperlink ref="B284" r:id="rId260"/>
-    <hyperlink ref="B285" r:id="rId261"/>
-    <hyperlink ref="B286" r:id="rId262"/>
-    <hyperlink ref="B287" r:id="rId263"/>
-    <hyperlink ref="B288" r:id="rId264"/>
-    <hyperlink ref="B289" r:id="rId265"/>
-    <hyperlink ref="B290" r:id="rId266"/>
-    <hyperlink ref="B291" r:id="rId267"/>
-    <hyperlink ref="B292" r:id="rId268"/>
-    <hyperlink ref="B293" r:id="rId269"/>
-    <hyperlink ref="B296" r:id="rId270"/>
-    <hyperlink ref="B297" r:id="rId271"/>
-    <hyperlink ref="B298" r:id="rId272"/>
-    <hyperlink ref="B299" r:id="rId273"/>
-    <hyperlink ref="B300" r:id="rId274"/>
-    <hyperlink ref="B301" r:id="rId275"/>
-    <hyperlink ref="B302" r:id="rId276"/>
-    <hyperlink ref="B303" r:id="rId277"/>
-    <hyperlink ref="B304" r:id="rId278"/>
-    <hyperlink ref="B305" r:id="rId279"/>
-    <hyperlink ref="B306" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
-    <hyperlink ref="B307" r:id="rId281"/>
-    <hyperlink ref="B308" r:id="rId282"/>
-    <hyperlink ref="B309" r:id="rId283"/>
-    <hyperlink ref="B310" r:id="rId284"/>
-    <hyperlink ref="B311" r:id="rId285"/>
-    <hyperlink ref="B312" r:id="rId286"/>
-    <hyperlink ref="B313" r:id="rId287"/>
-    <hyperlink ref="B314" r:id="rId288"/>
-    <hyperlink ref="B315" r:id="rId289"/>
-    <hyperlink ref="B316" r:id="rId290"/>
-    <hyperlink ref="B317" r:id="rId291"/>
-    <hyperlink ref="B318" r:id="rId292"/>
-    <hyperlink ref="B319" r:id="rId293"/>
-    <hyperlink ref="B320" r:id="rId294"/>
-    <hyperlink ref="B321" r:id="rId295"/>
-    <hyperlink ref="B322" r:id="rId296"/>
-    <hyperlink ref="B323" r:id="rId297"/>
-    <hyperlink ref="B324" r:id="rId298"/>
-    <hyperlink ref="B325" r:id="rId299"/>
-    <hyperlink ref="B326" r:id="rId300"/>
-    <hyperlink ref="B327" r:id="rId301"/>
-    <hyperlink ref="B328" r:id="rId302"/>
-    <hyperlink ref="B329" r:id="rId303"/>
-    <hyperlink ref="B330" r:id="rId304"/>
-    <hyperlink ref="B331" r:id="rId305"/>
-    <hyperlink ref="B332" r:id="rId306"/>
-    <hyperlink ref="B333" r:id="rId307"/>
-    <hyperlink ref="B336" r:id="rId308"/>
-    <hyperlink ref="B337" r:id="rId309"/>
-    <hyperlink ref="B338" r:id="rId310"/>
-    <hyperlink ref="B339" r:id="rId311"/>
-    <hyperlink ref="B340" r:id="rId312"/>
-    <hyperlink ref="B341" r:id="rId313"/>
-    <hyperlink ref="B342" r:id="rId314"/>
-    <hyperlink ref="B343" r:id="rId315"/>
-    <hyperlink ref="B344" r:id="rId316"/>
-    <hyperlink ref="B345" r:id="rId317"/>
-    <hyperlink ref="B346" r:id="rId318"/>
-    <hyperlink ref="B347" r:id="rId319"/>
-    <hyperlink ref="B348" r:id="rId320"/>
-    <hyperlink ref="B349" r:id="rId321"/>
-    <hyperlink ref="B350" r:id="rId322"/>
-    <hyperlink ref="B351" r:id="rId323"/>
-    <hyperlink ref="B352" r:id="rId324"/>
-    <hyperlink ref="B353" r:id="rId325"/>
-    <hyperlink ref="B357" r:id="rId326"/>
-    <hyperlink ref="B358" r:id="rId327"/>
-    <hyperlink ref="B359" r:id="rId328"/>
-    <hyperlink ref="B360" r:id="rId329"/>
-    <hyperlink ref="B361" r:id="rId330"/>
-    <hyperlink ref="B362" r:id="rId331"/>
-    <hyperlink ref="B363" r:id="rId332"/>
-    <hyperlink ref="B364" r:id="rId333"/>
-    <hyperlink ref="B365" r:id="rId334"/>
-    <hyperlink ref="B366" r:id="rId335"/>
-    <hyperlink ref="B367" r:id="rId336"/>
-    <hyperlink ref="B368" r:id="rId337"/>
-    <hyperlink ref="B369" r:id="rId338"/>
-    <hyperlink ref="B370" r:id="rId339"/>
-    <hyperlink ref="B371" r:id="rId340"/>
-    <hyperlink ref="B372" r:id="rId341"/>
-    <hyperlink ref="B373" r:id="rId342"/>
-    <hyperlink ref="B374" r:id="rId343"/>
-    <hyperlink ref="B375" r:id="rId344"/>
-    <hyperlink ref="B376" r:id="rId345"/>
-    <hyperlink ref="B377" r:id="rId346"/>
-    <hyperlink ref="B378" r:id="rId347"/>
-    <hyperlink ref="B379" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
-    <hyperlink ref="B380" r:id="rId349"/>
-    <hyperlink ref="B381" r:id="rId350"/>
-    <hyperlink ref="B382" r:id="rId351"/>
-    <hyperlink ref="B383" r:id="rId352"/>
-    <hyperlink ref="B384" r:id="rId353"/>
-    <hyperlink ref="B385" r:id="rId354"/>
-    <hyperlink ref="B386" r:id="rId355"/>
-    <hyperlink ref="B387" r:id="rId356"/>
-    <hyperlink ref="B388" r:id="rId357"/>
-    <hyperlink ref="B389" r:id="rId358"/>
-    <hyperlink ref="B390" r:id="rId359"/>
-    <hyperlink ref="B391" r:id="rId360"/>
-    <hyperlink ref="B392" r:id="rId361"/>
-    <hyperlink ref="B393" r:id="rId362"/>
-    <hyperlink ref="B394" r:id="rId363"/>
-    <hyperlink ref="B396" r:id="rId364"/>
-    <hyperlink ref="B395" r:id="rId365"/>
-    <hyperlink ref="B397" r:id="rId366"/>
-    <hyperlink ref="B398" r:id="rId367"/>
-    <hyperlink ref="B399" r:id="rId368"/>
-    <hyperlink ref="B402" r:id="rId369"/>
-    <hyperlink ref="B403" r:id="rId370"/>
-    <hyperlink ref="B404" r:id="rId371"/>
-    <hyperlink ref="B405" r:id="rId372"/>
-    <hyperlink ref="B406" r:id="rId373"/>
-    <hyperlink ref="B407" r:id="rId374"/>
-    <hyperlink ref="B410" r:id="rId375"/>
-    <hyperlink ref="B411" r:id="rId376"/>
-    <hyperlink ref="B412" r:id="rId377"/>
-    <hyperlink ref="B413" r:id="rId378"/>
-    <hyperlink ref="B414" r:id="rId379"/>
-    <hyperlink ref="B415" r:id="rId380"/>
-    <hyperlink ref="B416" r:id="rId381"/>
-    <hyperlink ref="B417" r:id="rId382"/>
-    <hyperlink ref="B418" r:id="rId383"/>
-    <hyperlink ref="B419" r:id="rId384"/>
-    <hyperlink ref="B420" r:id="rId385"/>
-    <hyperlink ref="B421" r:id="rId386"/>
-    <hyperlink ref="B422" r:id="rId387"/>
-    <hyperlink ref="B423" r:id="rId388"/>
-    <hyperlink ref="B424" r:id="rId389"/>
-    <hyperlink ref="B425" r:id="rId390"/>
-    <hyperlink ref="B426" r:id="rId391"/>
-    <hyperlink ref="B427" r:id="rId392"/>
-    <hyperlink ref="B428" r:id="rId393"/>
-    <hyperlink ref="B429" r:id="rId394"/>
-    <hyperlink ref="B430" r:id="rId395"/>
-    <hyperlink ref="B431" r:id="rId396"/>
-    <hyperlink ref="B432" r:id="rId397"/>
-    <hyperlink ref="B433" r:id="rId398"/>
-    <hyperlink ref="B434" r:id="rId399"/>
-    <hyperlink ref="B435" r:id="rId400"/>
-    <hyperlink ref="B436" r:id="rId401"/>
-    <hyperlink ref="B437" r:id="rId402"/>
-    <hyperlink ref="B438" r:id="rId403"/>
-    <hyperlink ref="B439" r:id="rId404"/>
-    <hyperlink ref="B440" r:id="rId405"/>
-    <hyperlink ref="B441" r:id="rId406"/>
-    <hyperlink ref="B442" r:id="rId407"/>
-    <hyperlink ref="B443" r:id="rId408"/>
-    <hyperlink ref="B444" r:id="rId409"/>
-    <hyperlink ref="B445" r:id="rId410"/>
-    <hyperlink ref="B446" r:id="rId411"/>
-    <hyperlink ref="B447" r:id="rId412"/>
-    <hyperlink ref="B448" r:id="rId413"/>
-    <hyperlink ref="B449" r:id="rId414"/>
-    <hyperlink ref="B451" r:id="rId415"/>
-    <hyperlink ref="B450" r:id="rId416"/>
-    <hyperlink ref="B452" r:id="rId417"/>
-    <hyperlink ref="B453" r:id="rId418"/>
-    <hyperlink ref="B454" r:id="rId419"/>
-    <hyperlink ref="B455" r:id="rId420"/>
-    <hyperlink ref="B456" r:id="rId421"/>
-    <hyperlink ref="B457" r:id="rId422"/>
-    <hyperlink ref="B458" r:id="rId423"/>
-    <hyperlink ref="B459" r:id="rId424"/>
-    <hyperlink ref="B460" r:id="rId425"/>
-    <hyperlink ref="B461" r:id="rId426"/>
-    <hyperlink ref="B462" r:id="rId427"/>
-    <hyperlink ref="B469" r:id="rId428"/>
-    <hyperlink ref="B468" r:id="rId429"/>
-    <hyperlink ref="B467" r:id="rId430"/>
-    <hyperlink ref="B466" r:id="rId431"/>
-    <hyperlink ref="B465" r:id="rId432"/>
-    <hyperlink ref="B464" r:id="rId433"/>
-    <hyperlink ref="B463" r:id="rId434"/>
-    <hyperlink ref="B472" r:id="rId435"/>
-    <hyperlink ref="B473" r:id="rId436"/>
-    <hyperlink ref="B474" r:id="rId437"/>
-    <hyperlink ref="B475" r:id="rId438"/>
-    <hyperlink ref="B476" r:id="rId439"/>
-    <hyperlink ref="B477" r:id="rId440"/>
-    <hyperlink ref="B478" r:id="rId441"/>
-    <hyperlink ref="B481" r:id="rId442"/>
-    <hyperlink ref="B479" r:id="rId443"/>
-    <hyperlink ref="B480" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
-    <hyperlink ref="B356" r:id="rId445"/>
-    <hyperlink ref="B2" r:id="rId446"/>
+    <hyperlink ref="B15" r:id="rId9"/>
+    <hyperlink ref="B16" r:id="rId10"/>
+    <hyperlink ref="B17" r:id="rId11"/>
+    <hyperlink ref="B18" r:id="rId12"/>
+    <hyperlink ref="B19" r:id="rId13"/>
+    <hyperlink ref="B20" r:id="rId14"/>
+    <hyperlink ref="B21" r:id="rId15"/>
+    <hyperlink ref="B22" r:id="rId16"/>
+    <hyperlink ref="B23" r:id="rId17"/>
+    <hyperlink ref="B24" r:id="rId18"/>
+    <hyperlink ref="B25" r:id="rId19"/>
+    <hyperlink ref="B26" r:id="rId20"/>
+    <hyperlink ref="B27" r:id="rId21"/>
+    <hyperlink ref="B28" r:id="rId22"/>
+    <hyperlink ref="B29" r:id="rId23"/>
+    <hyperlink ref="B30" r:id="rId24"/>
+    <hyperlink ref="B31" r:id="rId25"/>
+    <hyperlink ref="B32" r:id="rId26"/>
+    <hyperlink ref="B33" r:id="rId27"/>
+    <hyperlink ref="B34" r:id="rId28"/>
+    <hyperlink ref="B35" r:id="rId29"/>
+    <hyperlink ref="B36" r:id="rId30"/>
+    <hyperlink ref="B37" r:id="rId31"/>
+    <hyperlink ref="B38" r:id="rId32"/>
+    <hyperlink ref="B39" r:id="rId33"/>
+    <hyperlink ref="B40" r:id="rId34"/>
+    <hyperlink ref="B41" r:id="rId35"/>
+    <hyperlink ref="B44" r:id="rId36"/>
+    <hyperlink ref="B45" r:id="rId37"/>
+    <hyperlink ref="B46" r:id="rId38"/>
+    <hyperlink ref="B47" r:id="rId39"/>
+    <hyperlink ref="B48" r:id="rId40"/>
+    <hyperlink ref="B49" r:id="rId41"/>
+    <hyperlink ref="B50" r:id="rId42"/>
+    <hyperlink ref="B51" r:id="rId43"/>
+    <hyperlink ref="B52" r:id="rId44"/>
+    <hyperlink ref="B53" r:id="rId45"/>
+    <hyperlink ref="B56" r:id="rId46"/>
+    <hyperlink ref="B57" r:id="rId47"/>
+    <hyperlink ref="B58" r:id="rId48"/>
+    <hyperlink ref="B60" r:id="rId49"/>
+    <hyperlink ref="B61" r:id="rId50"/>
+    <hyperlink ref="B62" r:id="rId51"/>
+    <hyperlink ref="B63" r:id="rId52"/>
+    <hyperlink ref="B64" r:id="rId53"/>
+    <hyperlink ref="B65" r:id="rId54"/>
+    <hyperlink ref="B66" r:id="rId55"/>
+    <hyperlink ref="B67" r:id="rId56"/>
+    <hyperlink ref="B68" r:id="rId57"/>
+    <hyperlink ref="B69" r:id="rId58"/>
+    <hyperlink ref="B70" r:id="rId59"/>
+    <hyperlink ref="B71" r:id="rId60"/>
+    <hyperlink ref="B72" r:id="rId61"/>
+    <hyperlink ref="B73" r:id="rId62"/>
+    <hyperlink ref="B74" r:id="rId63"/>
+    <hyperlink ref="B75" r:id="rId64"/>
+    <hyperlink ref="B76" r:id="rId65"/>
+    <hyperlink ref="B77" r:id="rId66"/>
+    <hyperlink ref="B78" r:id="rId67"/>
+    <hyperlink ref="B79" r:id="rId68"/>
+    <hyperlink ref="B80" r:id="rId69"/>
+    <hyperlink ref="B81" r:id="rId70"/>
+    <hyperlink ref="B82" r:id="rId71"/>
+    <hyperlink ref="B83" r:id="rId72"/>
+    <hyperlink ref="B84" r:id="rId73"/>
+    <hyperlink ref="B85" r:id="rId74"/>
+    <hyperlink ref="B86" r:id="rId75"/>
+    <hyperlink ref="B87" r:id="rId76"/>
+    <hyperlink ref="B88" r:id="rId77"/>
+    <hyperlink ref="B89" r:id="rId78"/>
+    <hyperlink ref="B90" r:id="rId79"/>
+    <hyperlink ref="B91" r:id="rId80"/>
+    <hyperlink ref="B92" r:id="rId81"/>
+    <hyperlink ref="B93" r:id="rId82"/>
+    <hyperlink ref="B94" r:id="rId83"/>
+    <hyperlink ref="B95" r:id="rId84"/>
+    <hyperlink ref="B96" r:id="rId85"/>
+    <hyperlink ref="B97" r:id="rId86"/>
+    <hyperlink ref="B98" r:id="rId87"/>
+    <hyperlink ref="B101" r:id="rId88"/>
+    <hyperlink ref="B102" r:id="rId89"/>
+    <hyperlink ref="B103" r:id="rId90"/>
+    <hyperlink ref="B104" r:id="rId91"/>
+    <hyperlink ref="B106" r:id="rId92" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance."/>
+    <hyperlink ref="B107" r:id="rId93"/>
+    <hyperlink ref="B108" r:id="rId94"/>
+    <hyperlink ref="B109" r:id="rId95"/>
+    <hyperlink ref="B110" r:id="rId96"/>
+    <hyperlink ref="B111" r:id="rId97"/>
+    <hyperlink ref="B113" r:id="rId98"/>
+    <hyperlink ref="B114" r:id="rId99"/>
+    <hyperlink ref="B115" r:id="rId100"/>
+    <hyperlink ref="B116" r:id="rId101"/>
+    <hyperlink ref="B117" r:id="rId102"/>
+    <hyperlink ref="B118" r:id="rId103"/>
+    <hyperlink ref="B119" r:id="rId104"/>
+    <hyperlink ref="B120" r:id="rId105"/>
+    <hyperlink ref="B121" r:id="rId106"/>
+    <hyperlink ref="B122" r:id="rId107"/>
+    <hyperlink ref="B123" r:id="rId108"/>
+    <hyperlink ref="B124" r:id="rId109"/>
+    <hyperlink ref="B125" r:id="rId110"/>
+    <hyperlink ref="B126" r:id="rId111"/>
+    <hyperlink ref="B127" r:id="rId112"/>
+    <hyperlink ref="B128" r:id="rId113"/>
+    <hyperlink ref="B129" r:id="rId114"/>
+    <hyperlink ref="B130" r:id="rId115"/>
+    <hyperlink ref="B131" r:id="rId116"/>
+    <hyperlink ref="B132" r:id="rId117"/>
+    <hyperlink ref="B133" r:id="rId118"/>
+    <hyperlink ref="B134" r:id="rId119"/>
+    <hyperlink ref="B135" r:id="rId120"/>
+    <hyperlink ref="B136" r:id="rId121"/>
+    <hyperlink ref="B105" r:id="rId122"/>
+    <hyperlink ref="B112" r:id="rId123"/>
+    <hyperlink ref="B139" r:id="rId124"/>
+    <hyperlink ref="B140" r:id="rId125"/>
+    <hyperlink ref="B141" r:id="rId126"/>
+    <hyperlink ref="B142" r:id="rId127"/>
+    <hyperlink ref="B143" r:id="rId128"/>
+    <hyperlink ref="B144" r:id="rId129"/>
+    <hyperlink ref="B145" r:id="rId130"/>
+    <hyperlink ref="B146" r:id="rId131"/>
+    <hyperlink ref="B147" r:id="rId132"/>
+    <hyperlink ref="B148" r:id="rId133"/>
+    <hyperlink ref="B149" r:id="rId134"/>
+    <hyperlink ref="B150" r:id="rId135"/>
+    <hyperlink ref="B151" r:id="rId136"/>
+    <hyperlink ref="B152" r:id="rId137"/>
+    <hyperlink ref="B153" r:id="rId138"/>
+    <hyperlink ref="B154" r:id="rId139"/>
+    <hyperlink ref="B155" r:id="rId140"/>
+    <hyperlink ref="B156" r:id="rId141"/>
+    <hyperlink ref="B157" r:id="rId142"/>
+    <hyperlink ref="B158" r:id="rId143"/>
+    <hyperlink ref="B159" r:id="rId144"/>
+    <hyperlink ref="B160" r:id="rId145"/>
+    <hyperlink ref="B161" r:id="rId146"/>
+    <hyperlink ref="B162" r:id="rId147"/>
+    <hyperlink ref="B163" r:id="rId148"/>
+    <hyperlink ref="B166" r:id="rId149"/>
+    <hyperlink ref="B167" r:id="rId150"/>
+    <hyperlink ref="B168" r:id="rId151"/>
+    <hyperlink ref="B169" r:id="rId152"/>
+    <hyperlink ref="B170" r:id="rId153"/>
+    <hyperlink ref="B171" r:id="rId154"/>
+    <hyperlink ref="B172" r:id="rId155"/>
+    <hyperlink ref="B173" r:id="rId156"/>
+    <hyperlink ref="B174" r:id="rId157"/>
+    <hyperlink ref="B177" r:id="rId158"/>
+    <hyperlink ref="B178" r:id="rId159"/>
+    <hyperlink ref="B179" r:id="rId160"/>
+    <hyperlink ref="B180" r:id="rId161"/>
+    <hyperlink ref="B181" r:id="rId162"/>
+    <hyperlink ref="B182" r:id="rId163"/>
+    <hyperlink ref="B183" r:id="rId164"/>
+    <hyperlink ref="B184" r:id="rId165"/>
+    <hyperlink ref="B185" r:id="rId166"/>
+    <hyperlink ref="B186" r:id="rId167"/>
+    <hyperlink ref="B187" r:id="rId168"/>
+    <hyperlink ref="B188" r:id="rId169"/>
+    <hyperlink ref="B189" r:id="rId170"/>
+    <hyperlink ref="B190" r:id="rId171"/>
+    <hyperlink ref="B191" r:id="rId172"/>
+    <hyperlink ref="B192" r:id="rId173"/>
+    <hyperlink ref="B193" r:id="rId174"/>
+    <hyperlink ref="B194" r:id="rId175"/>
+    <hyperlink ref="B195" r:id="rId176"/>
+    <hyperlink ref="B196" r:id="rId177"/>
+    <hyperlink ref="B197" r:id="rId178" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010."/>
+    <hyperlink ref="B198" r:id="rId179"/>
+    <hyperlink ref="B199" r:id="rId180"/>
+    <hyperlink ref="B200" r:id="rId181"/>
+    <hyperlink ref="B201" r:id="rId182"/>
+    <hyperlink ref="B202" r:id="rId183"/>
+    <hyperlink ref="B203" r:id="rId184" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not."/>
+    <hyperlink ref="B204" r:id="rId185"/>
+    <hyperlink ref="B205" r:id="rId186"/>
+    <hyperlink ref="B206" r:id="rId187"/>
+    <hyperlink ref="B207" r:id="rId188"/>
+    <hyperlink ref="B208" r:id="rId189"/>
+    <hyperlink ref="B209" r:id="rId190"/>
+    <hyperlink ref="B210" r:id="rId191"/>
+    <hyperlink ref="B211" r:id="rId192"/>
+    <hyperlink ref="B214" r:id="rId193"/>
+    <hyperlink ref="B215" r:id="rId194"/>
+    <hyperlink ref="B216" r:id="rId195"/>
+    <hyperlink ref="B217" r:id="rId196"/>
+    <hyperlink ref="B218" r:id="rId197"/>
+    <hyperlink ref="B219" r:id="rId198"/>
+    <hyperlink ref="B220" r:id="rId199"/>
+    <hyperlink ref="B221" r:id="rId200"/>
+    <hyperlink ref="B222" r:id="rId201"/>
+    <hyperlink ref="B223" r:id="rId202"/>
+    <hyperlink ref="B224" r:id="rId203"/>
+    <hyperlink ref="B225" r:id="rId204"/>
+    <hyperlink ref="B226" r:id="rId205"/>
+    <hyperlink ref="B227" r:id="rId206"/>
+    <hyperlink ref="B228" r:id="rId207"/>
+    <hyperlink ref="B229" r:id="rId208"/>
+    <hyperlink ref="B230" r:id="rId209"/>
+    <hyperlink ref="B231" r:id="rId210"/>
+    <hyperlink ref="B232" r:id="rId211"/>
+    <hyperlink ref="B233" r:id="rId212"/>
+    <hyperlink ref="B234" r:id="rId213"/>
+    <hyperlink ref="B235" r:id="rId214"/>
+    <hyperlink ref="B238" r:id="rId215"/>
+    <hyperlink ref="B239" r:id="rId216"/>
+    <hyperlink ref="B240" r:id="rId217"/>
+    <hyperlink ref="B241" r:id="rId218"/>
+    <hyperlink ref="B242" r:id="rId219"/>
+    <hyperlink ref="B243" r:id="rId220"/>
+    <hyperlink ref="B244" r:id="rId221"/>
+    <hyperlink ref="B245" r:id="rId222"/>
+    <hyperlink ref="B246" r:id="rId223"/>
+    <hyperlink ref="B247" r:id="rId224"/>
+    <hyperlink ref="B248" r:id="rId225"/>
+    <hyperlink ref="B249" r:id="rId226"/>
+    <hyperlink ref="B250" r:id="rId227"/>
+    <hyperlink ref="B251" r:id="rId228"/>
+    <hyperlink ref="B252" r:id="rId229"/>
+    <hyperlink ref="B253" r:id="rId230"/>
+    <hyperlink ref="B254" r:id="rId231"/>
+    <hyperlink ref="B255" r:id="rId232"/>
+    <hyperlink ref="B256" r:id="rId233"/>
+    <hyperlink ref="B257" r:id="rId234" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
+    <hyperlink ref="B258" r:id="rId235"/>
+    <hyperlink ref="B259" r:id="rId236"/>
+    <hyperlink ref="B260" r:id="rId237"/>
+    <hyperlink ref="B261" r:id="rId238"/>
+    <hyperlink ref="B262" r:id="rId239"/>
+    <hyperlink ref="B263" r:id="rId240"/>
+    <hyperlink ref="B264" r:id="rId241"/>
+    <hyperlink ref="B265" r:id="rId242"/>
+    <hyperlink ref="B266" r:id="rId243"/>
+    <hyperlink ref="B267" r:id="rId244"/>
+    <hyperlink ref="B268" r:id="rId245"/>
+    <hyperlink ref="B269" r:id="rId246"/>
+    <hyperlink ref="B270" r:id="rId247"/>
+    <hyperlink ref="B271" r:id="rId248"/>
+    <hyperlink ref="B272" r:id="rId249"/>
+    <hyperlink ref="B275" r:id="rId250"/>
+    <hyperlink ref="B276" r:id="rId251"/>
+    <hyperlink ref="B277" r:id="rId252"/>
+    <hyperlink ref="B278" r:id="rId253"/>
+    <hyperlink ref="B279" r:id="rId254"/>
+    <hyperlink ref="B280" r:id="rId255"/>
+    <hyperlink ref="B281" r:id="rId256"/>
+    <hyperlink ref="B282" r:id="rId257"/>
+    <hyperlink ref="B283" r:id="rId258"/>
+    <hyperlink ref="B284" r:id="rId259"/>
+    <hyperlink ref="B285" r:id="rId260"/>
+    <hyperlink ref="B286" r:id="rId261"/>
+    <hyperlink ref="B287" r:id="rId262"/>
+    <hyperlink ref="B288" r:id="rId263"/>
+    <hyperlink ref="B289" r:id="rId264"/>
+    <hyperlink ref="B290" r:id="rId265"/>
+    <hyperlink ref="B291" r:id="rId266"/>
+    <hyperlink ref="B292" r:id="rId267"/>
+    <hyperlink ref="B293" r:id="rId268"/>
+    <hyperlink ref="B296" r:id="rId269"/>
+    <hyperlink ref="B297" r:id="rId270"/>
+    <hyperlink ref="B298" r:id="rId271"/>
+    <hyperlink ref="B299" r:id="rId272"/>
+    <hyperlink ref="B300" r:id="rId273"/>
+    <hyperlink ref="B301" r:id="rId274"/>
+    <hyperlink ref="B302" r:id="rId275"/>
+    <hyperlink ref="B303" r:id="rId276"/>
+    <hyperlink ref="B304" r:id="rId277"/>
+    <hyperlink ref="B305" r:id="rId278"/>
+    <hyperlink ref="B306" r:id="rId279" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
+    <hyperlink ref="B307" r:id="rId280"/>
+    <hyperlink ref="B308" r:id="rId281"/>
+    <hyperlink ref="B309" r:id="rId282"/>
+    <hyperlink ref="B310" r:id="rId283"/>
+    <hyperlink ref="B311" r:id="rId284"/>
+    <hyperlink ref="B312" r:id="rId285"/>
+    <hyperlink ref="B313" r:id="rId286"/>
+    <hyperlink ref="B314" r:id="rId287"/>
+    <hyperlink ref="B315" r:id="rId288"/>
+    <hyperlink ref="B316" r:id="rId289"/>
+    <hyperlink ref="B317" r:id="rId290"/>
+    <hyperlink ref="B318" r:id="rId291"/>
+    <hyperlink ref="B319" r:id="rId292"/>
+    <hyperlink ref="B320" r:id="rId293"/>
+    <hyperlink ref="B321" r:id="rId294"/>
+    <hyperlink ref="B322" r:id="rId295"/>
+    <hyperlink ref="B323" r:id="rId296"/>
+    <hyperlink ref="B324" r:id="rId297"/>
+    <hyperlink ref="B325" r:id="rId298"/>
+    <hyperlink ref="B326" r:id="rId299"/>
+    <hyperlink ref="B327" r:id="rId300"/>
+    <hyperlink ref="B328" r:id="rId301"/>
+    <hyperlink ref="B329" r:id="rId302"/>
+    <hyperlink ref="B330" r:id="rId303"/>
+    <hyperlink ref="B331" r:id="rId304"/>
+    <hyperlink ref="B332" r:id="rId305"/>
+    <hyperlink ref="B333" r:id="rId306"/>
+    <hyperlink ref="B336" r:id="rId307"/>
+    <hyperlink ref="B337" r:id="rId308"/>
+    <hyperlink ref="B338" r:id="rId309"/>
+    <hyperlink ref="B339" r:id="rId310"/>
+    <hyperlink ref="B340" r:id="rId311"/>
+    <hyperlink ref="B341" r:id="rId312"/>
+    <hyperlink ref="B342" r:id="rId313"/>
+    <hyperlink ref="B343" r:id="rId314"/>
+    <hyperlink ref="B344" r:id="rId315"/>
+    <hyperlink ref="B345" r:id="rId316"/>
+    <hyperlink ref="B346" r:id="rId317"/>
+    <hyperlink ref="B347" r:id="rId318"/>
+    <hyperlink ref="B348" r:id="rId319"/>
+    <hyperlink ref="B349" r:id="rId320"/>
+    <hyperlink ref="B350" r:id="rId321"/>
+    <hyperlink ref="B351" r:id="rId322"/>
+    <hyperlink ref="B352" r:id="rId323"/>
+    <hyperlink ref="B353" r:id="rId324"/>
+    <hyperlink ref="B357" r:id="rId325"/>
+    <hyperlink ref="B358" r:id="rId326"/>
+    <hyperlink ref="B359" r:id="rId327"/>
+    <hyperlink ref="B360" r:id="rId328"/>
+    <hyperlink ref="B361" r:id="rId329"/>
+    <hyperlink ref="B362" r:id="rId330"/>
+    <hyperlink ref="B363" r:id="rId331"/>
+    <hyperlink ref="B364" r:id="rId332"/>
+    <hyperlink ref="B365" r:id="rId333"/>
+    <hyperlink ref="B366" r:id="rId334"/>
+    <hyperlink ref="B367" r:id="rId335"/>
+    <hyperlink ref="B368" r:id="rId336"/>
+    <hyperlink ref="B369" r:id="rId337"/>
+    <hyperlink ref="B370" r:id="rId338"/>
+    <hyperlink ref="B371" r:id="rId339"/>
+    <hyperlink ref="B372" r:id="rId340"/>
+    <hyperlink ref="B373" r:id="rId341"/>
+    <hyperlink ref="B374" r:id="rId342"/>
+    <hyperlink ref="B375" r:id="rId343"/>
+    <hyperlink ref="B376" r:id="rId344"/>
+    <hyperlink ref="B377" r:id="rId345"/>
+    <hyperlink ref="B378" r:id="rId346"/>
+    <hyperlink ref="B379" r:id="rId347" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
+    <hyperlink ref="B380" r:id="rId348"/>
+    <hyperlink ref="B381" r:id="rId349"/>
+    <hyperlink ref="B382" r:id="rId350"/>
+    <hyperlink ref="B383" r:id="rId351"/>
+    <hyperlink ref="B384" r:id="rId352"/>
+    <hyperlink ref="B385" r:id="rId353"/>
+    <hyperlink ref="B386" r:id="rId354"/>
+    <hyperlink ref="B387" r:id="rId355"/>
+    <hyperlink ref="B388" r:id="rId356"/>
+    <hyperlink ref="B389" r:id="rId357"/>
+    <hyperlink ref="B390" r:id="rId358"/>
+    <hyperlink ref="B391" r:id="rId359"/>
+    <hyperlink ref="B392" r:id="rId360"/>
+    <hyperlink ref="B393" r:id="rId361"/>
+    <hyperlink ref="B394" r:id="rId362"/>
+    <hyperlink ref="B396" r:id="rId363"/>
+    <hyperlink ref="B395" r:id="rId364"/>
+    <hyperlink ref="B397" r:id="rId365"/>
+    <hyperlink ref="B398" r:id="rId366"/>
+    <hyperlink ref="B399" r:id="rId367"/>
+    <hyperlink ref="B402" r:id="rId368"/>
+    <hyperlink ref="B403" r:id="rId369"/>
+    <hyperlink ref="B404" r:id="rId370"/>
+    <hyperlink ref="B405" r:id="rId371"/>
+    <hyperlink ref="B406" r:id="rId372"/>
+    <hyperlink ref="B407" r:id="rId373"/>
+    <hyperlink ref="B410" r:id="rId374"/>
+    <hyperlink ref="B411" r:id="rId375"/>
+    <hyperlink ref="B412" r:id="rId376"/>
+    <hyperlink ref="B413" r:id="rId377"/>
+    <hyperlink ref="B414" r:id="rId378"/>
+    <hyperlink ref="B415" r:id="rId379"/>
+    <hyperlink ref="B416" r:id="rId380"/>
+    <hyperlink ref="B417" r:id="rId381"/>
+    <hyperlink ref="B418" r:id="rId382"/>
+    <hyperlink ref="B419" r:id="rId383"/>
+    <hyperlink ref="B420" r:id="rId384"/>
+    <hyperlink ref="B421" r:id="rId385"/>
+    <hyperlink ref="B422" r:id="rId386"/>
+    <hyperlink ref="B423" r:id="rId387"/>
+    <hyperlink ref="B424" r:id="rId388"/>
+    <hyperlink ref="B425" r:id="rId389"/>
+    <hyperlink ref="B426" r:id="rId390"/>
+    <hyperlink ref="B427" r:id="rId391"/>
+    <hyperlink ref="B428" r:id="rId392"/>
+    <hyperlink ref="B429" r:id="rId393"/>
+    <hyperlink ref="B430" r:id="rId394"/>
+    <hyperlink ref="B431" r:id="rId395"/>
+    <hyperlink ref="B432" r:id="rId396"/>
+    <hyperlink ref="B433" r:id="rId397"/>
+    <hyperlink ref="B434" r:id="rId398"/>
+    <hyperlink ref="B435" r:id="rId399"/>
+    <hyperlink ref="B436" r:id="rId400"/>
+    <hyperlink ref="B437" r:id="rId401"/>
+    <hyperlink ref="B438" r:id="rId402"/>
+    <hyperlink ref="B439" r:id="rId403"/>
+    <hyperlink ref="B440" r:id="rId404"/>
+    <hyperlink ref="B441" r:id="rId405"/>
+    <hyperlink ref="B442" r:id="rId406"/>
+    <hyperlink ref="B443" r:id="rId407"/>
+    <hyperlink ref="B444" r:id="rId408"/>
+    <hyperlink ref="B445" r:id="rId409"/>
+    <hyperlink ref="B446" r:id="rId410"/>
+    <hyperlink ref="B447" r:id="rId411"/>
+    <hyperlink ref="B448" r:id="rId412"/>
+    <hyperlink ref="B449" r:id="rId413"/>
+    <hyperlink ref="B451" r:id="rId414"/>
+    <hyperlink ref="B450" r:id="rId415"/>
+    <hyperlink ref="B452" r:id="rId416"/>
+    <hyperlink ref="B453" r:id="rId417"/>
+    <hyperlink ref="B454" r:id="rId418"/>
+    <hyperlink ref="B455" r:id="rId419"/>
+    <hyperlink ref="B456" r:id="rId420"/>
+    <hyperlink ref="B457" r:id="rId421"/>
+    <hyperlink ref="B458" r:id="rId422"/>
+    <hyperlink ref="B459" r:id="rId423"/>
+    <hyperlink ref="B460" r:id="rId424"/>
+    <hyperlink ref="B461" r:id="rId425"/>
+    <hyperlink ref="B462" r:id="rId426"/>
+    <hyperlink ref="B469" r:id="rId427"/>
+    <hyperlink ref="B468" r:id="rId428"/>
+    <hyperlink ref="B467" r:id="rId429"/>
+    <hyperlink ref="B466" r:id="rId430"/>
+    <hyperlink ref="B465" r:id="rId431"/>
+    <hyperlink ref="B464" r:id="rId432"/>
+    <hyperlink ref="B463" r:id="rId433"/>
+    <hyperlink ref="B472" r:id="rId434"/>
+    <hyperlink ref="B473" r:id="rId435"/>
+    <hyperlink ref="B474" r:id="rId436"/>
+    <hyperlink ref="B475" r:id="rId437"/>
+    <hyperlink ref="B476" r:id="rId438"/>
+    <hyperlink ref="B477" r:id="rId439"/>
+    <hyperlink ref="B478" r:id="rId440"/>
+    <hyperlink ref="B481" r:id="rId441"/>
+    <hyperlink ref="B479" r:id="rId442"/>
+    <hyperlink ref="B480" r:id="rId443" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
+    <hyperlink ref="B356" r:id="rId444"/>
+    <hyperlink ref="B2" r:id="rId445"/>
+    <hyperlink ref="B14" r:id="rId446"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId447"/>

</xml_diff>

<commit_message>
63 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1858,7 +1858,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2789,7 +2789,7 @@
         <v>87</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="21">
@@ -3326,7 +3326,7 @@
         <v>137</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="21">
@@ -3337,7 +3337,7 @@
         <v>138</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="21">
@@ -3348,7 +3348,7 @@
         <v>139</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="21">
@@ -3370,7 +3370,7 @@
         <v>141</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="21">

</xml_diff>

<commit_message>
66 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A423" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B430" sqref="B430"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3436,7 +3436,7 @@
         <v>147</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="21">
@@ -3458,7 +3458,7 @@
         <v>149</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="21">
@@ -3935,7 +3935,7 @@
         <v>193</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="21">

</xml_diff>

<commit_message>
71 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A423" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B430" sqref="B430"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6157,7 +6157,7 @@
         <v>394</v>
       </c>
       <c r="C410" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="411" spans="1:3" ht="21">
@@ -6168,7 +6168,7 @@
         <v>395</v>
       </c>
       <c r="C411" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="412" spans="1:3" ht="21">
@@ -6223,7 +6223,7 @@
         <v>400</v>
       </c>
       <c r="C416" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="417" spans="1:3" ht="21">
@@ -6234,7 +6234,7 @@
         <v>273</v>
       </c>
       <c r="C417" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="418" spans="1:3" ht="21">
@@ -6300,7 +6300,7 @@
         <v>406</v>
       </c>
       <c r="C423" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="424" spans="1:3" ht="21">

</xml_diff>

<commit_message>
77 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2866,7 +2866,7 @@
         <v>94</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="21">
@@ -2877,7 +2877,7 @@
         <v>95</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="21">
@@ -3447,7 +3447,7 @@
         <v>148</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="21">
@@ -3469,7 +3469,7 @@
         <v>150</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="21">
@@ -5047,7 +5047,7 @@
         <v>294</v>
       </c>
       <c r="C304" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="305" spans="1:3" ht="21">
@@ -5418,7 +5418,7 @@
         <v>328</v>
       </c>
       <c r="C339" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="340" spans="1:3" ht="21">

</xml_diff>

<commit_message>
80 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2023,7 +2023,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="21">
@@ -2056,7 +2056,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="21">
@@ -2133,7 +2133,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="21">

</xml_diff>

<commit_message>
86 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2926,7 +2926,7 @@
         <v>100</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="21">
@@ -3381,7 +3381,7 @@
         <v>142</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="21">
@@ -3392,7 +3392,7 @@
         <v>143</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="21">
@@ -3612,7 +3612,7 @@
         <v>163</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="21">
@@ -3979,7 +3979,7 @@
         <v>197</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="21">
@@ -4690,7 +4690,7 @@
         <v>262</v>
       </c>
       <c r="C269" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="270" spans="1:3" ht="21">

</xml_diff>

<commit_message>
89 of 450 question done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2144,7 +2144,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="21">
@@ -2210,7 +2210,7 @@
         <v>34</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="21">
@@ -4132,7 +4132,7 @@
         <v>211</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="21">

</xml_diff>

<commit_message>
93 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A221" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B229" sqref="B229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6179,7 +6179,7 @@
         <v>396</v>
       </c>
       <c r="C412" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="413" spans="1:3" ht="21">
@@ -6311,7 +6311,7 @@
         <v>407</v>
       </c>
       <c r="C424" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="425" spans="1:3" ht="21">
@@ -6498,7 +6498,7 @@
         <v>424</v>
       </c>
       <c r="C441" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="442" spans="1:3" ht="21">
@@ -6806,7 +6806,7 @@
         <v>452</v>
       </c>
       <c r="C469" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="470" spans="1:3" ht="21">

</xml_diff>

<commit_message>
98 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A221" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B229" sqref="B229"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1979,7 +1979,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21">
@@ -2034,7 +2034,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21">
@@ -3513,7 +3513,7 @@
         <v>154</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="21">
@@ -4264,7 +4264,7 @@
         <v>223</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="21">
@@ -4330,7 +4330,7 @@
         <v>229</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="236" spans="1:3" ht="21">

</xml_diff>

<commit_message>
102 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1946,7 +1946,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21">
@@ -1957,7 +1957,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21">
@@ -1968,7 +1968,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="21">
@@ -1990,7 +1990,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="21">

</xml_diff>

<commit_message>
108 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1858,7 +1858,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3737,7 +3737,7 @@
         <v>175</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="21">
@@ -3858,7 +3858,7 @@
         <v>186</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="21">
@@ -4349,7 +4349,7 @@
         <v>231</v>
       </c>
       <c r="C238" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="21">
@@ -4819,7 +4819,7 @@
         <v>273</v>
       </c>
       <c r="C282" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="283" spans="1:3" ht="21">
@@ -5602,7 +5602,7 @@
         <v>345</v>
       </c>
       <c r="C357" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="358" spans="1:3" ht="21">
@@ -5613,7 +5613,7 @@
         <v>346</v>
       </c>
       <c r="C358" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="359" spans="1:3" ht="21">

</xml_diff>

<commit_message>
113 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1858,7 +1858,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2800,7 +2800,7 @@
         <v>88</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="21">
@@ -2811,7 +2811,7 @@
         <v>89</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="21">
@@ -5517,7 +5517,7 @@
         <v>337</v>
       </c>
       <c r="C348" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="349" spans="1:3" ht="21">
@@ -5646,7 +5646,7 @@
         <v>349</v>
       </c>
       <c r="C361" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="362" spans="1:3" ht="21">
@@ -5756,7 +5756,7 @@
         <v>359</v>
       </c>
       <c r="C371" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="372" spans="1:3" ht="21">

</xml_diff>

<commit_message>
117 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1858,7 +1858,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4742,7 +4742,7 @@
         <v>266</v>
       </c>
       <c r="C275" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="276" spans="1:3" ht="21">
@@ -5635,7 +5635,7 @@
         <v>348</v>
       </c>
       <c r="C360" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="361" spans="1:3" ht="21">
@@ -5723,7 +5723,7 @@
         <v>356</v>
       </c>
       <c r="C368" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="369" spans="1:3" ht="21">
@@ -6476,7 +6476,7 @@
         <v>422</v>
       </c>
       <c r="C439" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="440" spans="1:3" ht="21">

</xml_diff>

<commit_message>
121 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A436" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B477" sqref="B477"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2078,7 +2078,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21">
@@ -2089,7 +2089,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="21">
@@ -2470,7 +2470,7 @@
         <v>58</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="21">
@@ -5135,7 +5135,7 @@
         <v>302</v>
       </c>
       <c r="C312" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="313" spans="1:3" ht="21">

</xml_diff>

<commit_message>
127 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A436" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B477" sqref="B477"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2668,7 +2668,7 @@
         <v>76</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="21">
@@ -3414,7 +3414,7 @@
         <v>145</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="21">
@@ -5322,7 +5322,7 @@
         <v>319</v>
       </c>
       <c r="C329" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="330" spans="1:3" ht="21">
@@ -5440,7 +5440,7 @@
         <v>330</v>
       </c>
       <c r="C341" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="342" spans="1:3" ht="21">
@@ -5462,7 +5462,7 @@
         <v>332</v>
       </c>
       <c r="C343" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="344" spans="1:3" ht="21">
@@ -6245,7 +6245,7 @@
         <v>401</v>
       </c>
       <c r="C418" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="419" spans="1:3" ht="21">

</xml_diff>

<commit_message>
132 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2122,7 +2122,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="21">
@@ -2177,7 +2177,7 @@
         <v>31</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="21">
@@ -2970,7 +2970,7 @@
         <v>104</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="21">
@@ -3003,7 +3003,7 @@
         <v>107</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="21">
@@ -3425,7 +3425,7 @@
         <v>146</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="21">

</xml_diff>

<commit_message>
135 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1858,7 +1858,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2366,7 +2366,7 @@
         <v>48</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="21">
@@ -5624,7 +5624,7 @@
         <v>347</v>
       </c>
       <c r="C359" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="360" spans="1:3" ht="21">
@@ -5668,7 +5668,7 @@
         <v>351</v>
       </c>
       <c r="C363" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="364" spans="1:3" ht="21">

</xml_diff>

<commit_message>
142 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1858,7 +1858,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2045,7 +2045,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21">
@@ -2322,7 +2322,7 @@
         <v>44</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="21">
@@ -2344,7 +2344,7 @@
         <v>46</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="21">
@@ -2377,7 +2377,7 @@
         <v>49</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="21">
@@ -2514,7 +2514,7 @@
         <v>62</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="21">
@@ -2525,7 +2525,7 @@
         <v>63</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="21">
@@ -2580,7 +2580,7 @@
         <v>68</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="21">

</xml_diff>

<commit_message>
144 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="C156" sqref="C156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2311,7 +2311,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="21">
@@ -3491,7 +3491,7 @@
         <v>152</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="21">

</xml_diff>

<commit_message>
149 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="C156" sqref="C156"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2591,7 +2591,7 @@
         <v>69</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="21">
@@ -2937,7 +2937,7 @@
         <v>101</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="21">
@@ -4067,7 +4067,7 @@
         <v>205</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="211" spans="1:3" ht="21">
@@ -4078,7 +4078,7 @@
         <v>206</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="212" spans="1:3" ht="21">
@@ -5080,7 +5080,7 @@
         <v>297</v>
       </c>
       <c r="C307" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="308" spans="1:3" ht="21">

</xml_diff>

<commit_message>
153 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1858,7 +1858,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2012,7 +2012,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21">
@@ -2265,7 +2265,7 @@
         <v>39</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="21">
@@ -3025,7 +3025,7 @@
         <v>109</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="21">
@@ -3990,7 +3990,7 @@
         <v>198</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="21">

</xml_diff>

<commit_message>
155 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1858,7 +1858,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4602,7 +4602,7 @@
         <v>254</v>
       </c>
       <c r="C261" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="262" spans="1:3" ht="21">
@@ -6322,7 +6322,7 @@
         <v>408</v>
       </c>
       <c r="C425" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="426" spans="1:3" ht="21">

</xml_diff>

<commit_message>
160 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="469">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1426,6 +1426,15 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>on GFG practice platform</t>
+  </si>
+  <si>
+    <t>On GFG practice</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -1847,7 +1856,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1855,10 +1864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C481"/>
+  <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A213" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1866,6 +1875,7 @@
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="23.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25">
@@ -2869,7 +2879,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="21">
+    <row r="97" spans="1:4" ht="21">
       <c r="A97" s="5" t="s">
         <v>53</v>
       </c>
@@ -2880,7 +2890,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="21">
+    <row r="98" spans="1:4" ht="21">
       <c r="A98" s="5" t="s">
         <v>53</v>
       </c>
@@ -2891,12 +2901,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="21">
+    <row r="100" spans="1:4" ht="21">
       <c r="A100" s="8"/>
       <c r="B100" s="7"/>
       <c r="C100" s="4"/>
     </row>
-    <row r="101" spans="1:3" ht="21">
+    <row r="101" spans="1:4" ht="21">
       <c r="A101" s="5" t="s">
         <v>97</v>
       </c>
@@ -2907,7 +2917,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="21">
+    <row r="102" spans="1:4" ht="21">
       <c r="A102" s="5" t="s">
         <v>97</v>
       </c>
@@ -2915,10 +2925,13 @@
         <v>99</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="21">
+        <v>468</v>
+      </c>
+      <c r="D102" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="21">
       <c r="A103" s="5" t="s">
         <v>97</v>
       </c>
@@ -2929,7 +2942,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="21">
+    <row r="104" spans="1:4" ht="21">
       <c r="A104" s="5" t="s">
         <v>97</v>
       </c>
@@ -2940,7 +2953,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="21">
+    <row r="105" spans="1:4" ht="21">
       <c r="A105" s="5" t="s">
         <v>97</v>
       </c>
@@ -2951,7 +2964,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="21">
+    <row r="106" spans="1:4" ht="21">
       <c r="A106" s="5" t="s">
         <v>97</v>
       </c>
@@ -2962,7 +2975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="21">
+    <row r="107" spans="1:4" ht="21">
       <c r="A107" s="5" t="s">
         <v>97</v>
       </c>
@@ -2973,7 +2986,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="21">
+    <row r="108" spans="1:4" ht="21">
       <c r="A108" s="5" t="s">
         <v>97</v>
       </c>
@@ -2984,7 +2997,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="21">
+    <row r="109" spans="1:4" ht="21">
       <c r="A109" s="5" t="s">
         <v>97</v>
       </c>
@@ -2995,7 +3008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="21">
+    <row r="110" spans="1:4" ht="21">
       <c r="A110" s="5" t="s">
         <v>97</v>
       </c>
@@ -3006,7 +3019,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="21">
+    <row r="111" spans="1:4" ht="21">
       <c r="A111" s="5" t="s">
         <v>97</v>
       </c>
@@ -3017,7 +3030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="21">
+    <row r="112" spans="1:4" ht="21">
       <c r="A112" s="5" t="s">
         <v>97</v>
       </c>
@@ -3146,7 +3159,7 @@
         <v>120</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="21">
@@ -3538,7 +3551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="21">
+    <row r="161" spans="1:4" ht="21">
       <c r="A161" s="8" t="s">
         <v>134</v>
       </c>
@@ -3549,7 +3562,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="21">
+    <row r="162" spans="1:4" ht="21">
       <c r="A162" s="8" t="s">
         <v>134</v>
       </c>
@@ -3560,7 +3573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="21">
+    <row r="163" spans="1:4" ht="21">
       <c r="A163" s="8" t="s">
         <v>134</v>
       </c>
@@ -3571,7 +3584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="21">
+    <row r="164" spans="1:4" ht="21">
       <c r="A164" s="8" t="s">
         <v>134</v>
       </c>
@@ -3582,7 +3595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="21">
+    <row r="165" spans="1:4" ht="21">
       <c r="A165" s="8" t="s">
         <v>134</v>
       </c>
@@ -3593,7 +3606,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="21">
+    <row r="166" spans="1:4" ht="21">
       <c r="A166" s="8" t="s">
         <v>134</v>
       </c>
@@ -3604,7 +3617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="21">
+    <row r="167" spans="1:4" ht="21">
       <c r="A167" s="8" t="s">
         <v>134</v>
       </c>
@@ -3615,7 +3628,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="21">
+    <row r="168" spans="1:4" ht="21">
       <c r="A168" s="8" t="s">
         <v>134</v>
       </c>
@@ -3623,10 +3636,13 @@
         <v>164</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" ht="21">
+        <v>465</v>
+      </c>
+      <c r="D168" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="21">
       <c r="A169" s="8" t="s">
         <v>134</v>
       </c>
@@ -3637,7 +3653,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="21">
+    <row r="170" spans="1:4" ht="21">
       <c r="A170" s="8" t="s">
         <v>134</v>
       </c>
@@ -3648,7 +3664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="21">
+    <row r="171" spans="1:4" ht="21">
       <c r="A171" s="8" t="s">
         <v>134</v>
       </c>
@@ -3659,7 +3675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="21">
+    <row r="172" spans="1:4" ht="21">
       <c r="A172" s="8" t="s">
         <v>134</v>
       </c>
@@ -3670,7 +3686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="21">
+    <row r="173" spans="1:4" ht="21">
       <c r="A173" s="8" t="s">
         <v>134</v>
       </c>
@@ -3681,7 +3697,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="21">
+    <row r="174" spans="1:4" ht="21">
       <c r="A174" s="8" t="s">
         <v>134</v>
       </c>
@@ -3689,10 +3705,10 @@
         <v>170</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" ht="21">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" ht="21">
       <c r="B176" s="7"/>
       <c r="C176" s="4"/>
     </row>
@@ -4712,7 +4728,7 @@
         <v>87</v>
       </c>
       <c r="C271" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="272" spans="1:3" ht="21">

</xml_diff>

<commit_message>
166 of 450 questions done
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1866,8 +1866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A213" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2612,7 +2612,7 @@
         <v>70</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="21">
@@ -4409,7 +4409,7 @@
         <v>235</v>
       </c>
       <c r="C242" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="243" spans="1:3" ht="21">
@@ -4442,7 +4442,7 @@
         <v>238</v>
       </c>
       <c r="C245" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="246" spans="1:3" ht="21">
@@ -4508,7 +4508,7 @@
         <v>244</v>
       </c>
       <c r="C251" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="252" spans="1:3" ht="21">
@@ -5030,7 +5030,7 @@
         <v>291</v>
       </c>
       <c r="C301" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="302" spans="1:3" ht="21">
@@ -5305,7 +5305,7 @@
         <v>316</v>
       </c>
       <c r="C326" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="327" spans="1:3" ht="21">

</xml_diff>

<commit_message>
168 of 450 questions & some imp questions
</commit_message>
<xml_diff>
--- a/build/classes/asset/DSA-450.xlsx
+++ b/build/classes/asset/DSA-450.xlsx
@@ -1856,7 +1856,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1867,7 +1867,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3929,7 +3929,7 @@
         <v>191</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="21">
@@ -5250,7 +5250,7 @@
         <v>311</v>
       </c>
       <c r="C321" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="322" spans="1:3" ht="21">

</xml_diff>